<commit_message>
updates levels in trap metadata xlsx
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_trap_metadata.xlsx
+++ b/data-raw/metadata/feather_trap_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-feather-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A53F9F9-611A-BD46-B421-61E24A078F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AADF9BFC-5DFF-EB4B-8C44-6E86D951D830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-21100" windowWidth="31680" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,13 +97,7 @@
     <t>siteName</t>
   </si>
   <si>
-    <t>Name of the sampling site</t>
-  </si>
-  <si>
     <t>subSiteName</t>
-  </si>
-  <si>
-    <t>Position of trap within the site</t>
   </si>
   <si>
     <t>visitTime</t>
@@ -127,13 +121,7 @@
     <t>fishProcessed</t>
   </si>
   <si>
-    <t>Describing if fish processed during trap visit</t>
-  </si>
-  <si>
     <t>trapFunctioning</t>
-  </si>
-  <si>
-    <t>Code for description of how well trap is functioning when visit to trap began</t>
   </si>
   <si>
     <t>counterAtEnd</t>
@@ -167,9 +155,6 @@
   </si>
   <si>
     <t>includeCatch</t>
-  </si>
-  <si>
-    <t>Code for whether this record is considered of high enough quality to include in analysis</t>
   </si>
   <si>
     <t>discharge</t>
@@ -215,6 +200,21 @@
   </si>
   <si>
     <t>attribute_name</t>
+  </si>
+  <si>
+    <t>Name of the sampling site. Levels = c("Eye Riffle", "Live Oak", "Herringer Riffle", "Steep Riffle", "Sunset Pumps", "Shawn's Beach", "Gateway Riffle")</t>
+  </si>
+  <si>
+    <t>Position of trap within the site. Levels = c("Eye riffle_north", "Live Oak", "Herringer_west”,” Herringer_east”, "Eye riffle_Side Channel”, “#Steep Riffle_RST”, “Sunset West bank”, "Sunset East bank”,” Shawns_west", "Shawns_east”, “Gateway_main1”, “Herringer_Upper_west”, “Steep Riffle_10' ext”, “Gateway Main 400' Up River”, “Gateway_Rootball”, “Steep Side Channel", “Gateway_Rootball_River_Left")</t>
+  </si>
+  <si>
+    <t>Describing if fish processed during trap visit. Levels = c("Not applicable", "Processed fish", "No fish were caught", "No catch data; fish released", "No catch data; fish left in live box")</t>
+  </si>
+  <si>
+    <t>Code for description of how well trap is functioning when visit to trap began. Levels = c("Trap not in service", "Not recorded", "Trap functioning normally", "Trap stopped functioning", "Trap functioning, but not normally")</t>
+  </si>
+  <si>
+    <t>Code for whether this record is considered of high enough quality to include in analysis. Levels = c("Yes", "No")</t>
   </si>
 </sst>
 </file>
@@ -546,7 +546,7 @@
   <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -698,26 +698,26 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="2"/>
       <c r="J4" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K4" s="10"/>
       <c r="L4" s="11"/>
@@ -741,7 +741,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
@@ -776,10 +776,10 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>19</v>
@@ -814,10 +814,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
@@ -852,10 +852,10 @@
     </row>
     <row r="8" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
@@ -890,10 +890,10 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
@@ -928,28 +928,28 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="3"/>
@@ -972,28 +972,28 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="3"/>
@@ -1016,28 +1016,28 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
@@ -1060,10 +1060,10 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>15</v>
@@ -1098,28 +1098,28 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="3"/>
@@ -1142,28 +1142,28 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="3"/>
@@ -1186,28 +1186,28 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="3"/>
@@ -1230,28 +1230,28 @@
     </row>
     <row r="17" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
@@ -28950,13 +28950,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>

</xml_diff>